<commit_message>
change multiple terminal messages type
</commit_message>
<xml_diff>
--- a/sheets/master_data.xlsx
+++ b/sheets/master_data.xlsx
@@ -298,10 +298,10 @@
     <xf numFmtId="0" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1752,7 +1752,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s" s="5">
         <v>14</v>
@@ -1765,7 +1765,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s" s="5">
         <v>15</v>
@@ -1778,7 +1778,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s" s="5">
         <v>16</v>
@@ -1791,7 +1791,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s" s="5">
         <v>17</v>
@@ -1804,7 +1804,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s" s="5">
         <v>18</v>
@@ -1817,7 +1817,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s" s="5">
         <v>19</v>
@@ -2207,7 +2207,7 @@
         <v>23</v>
       </c>
       <c r="B37" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C37" t="s" s="5">
         <v>48</v>
@@ -2220,7 +2220,7 @@
         <v>24</v>
       </c>
       <c r="B38" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s" s="5">
         <v>49</v>
@@ -2233,7 +2233,7 @@
         <v>25</v>
       </c>
       <c r="B39" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C39" t="s" s="5">
         <v>50</v>
@@ -2246,7 +2246,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C40" t="s" s="5">
         <v>51</v>
@@ -2259,7 +2259,7 @@
         <v>27</v>
       </c>
       <c r="B41" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s" s="5">
         <v>52</v>

</xml_diff>

<commit_message>
add change state action by master
</commit_message>
<xml_diff>
--- a/sheets/master_data.xlsx
+++ b/sheets/master_data.xlsx
@@ -279,7 +279,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -302,6 +302,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1720,7 +1723,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2267,6 +2270,17 @@
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
     </row>
+    <row r="42" ht="20" customHeight="1">
+      <c r="A42" s="5">
+        <v>28</v>
+      </c>
+      <c r="B42" s="5">
+        <v>4</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>

</xml_diff>